<commit_message>
New file and modification to Ins Understanding
</commit_message>
<xml_diff>
--- a/Insurance Understanding.xlsx
+++ b/Insurance Understanding.xlsx
@@ -5,19 +5,21 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Reporting\Insurance Reporting Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arun\Documents\GitHub\Insurance\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="TLI" sheetId="3" r:id="rId2"/>
     <sheet name="CI" sheetId="4" r:id="rId3"/>
     <sheet name="HI" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511" iterateCount="10" calcOnSave="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -301,7 +303,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1950" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1988" uniqueCount="155">
   <si>
     <t>visit</t>
   </si>
@@ -685,6 +687,87 @@
   </si>
   <si>
     <t xml:space="preserve">process understanding </t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Smoke/</t>
+  </si>
+  <si>
+    <t>Applicant City</t>
+  </si>
+  <si>
+    <t>Gross Mn</t>
+  </si>
+  <si>
+    <t>CI</t>
+  </si>
+  <si>
+    <t>TLI</t>
+  </si>
+  <si>
+    <t>Dimensions at eligibiity Page</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Appl Dimension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of </t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>Raise Reqest</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>uniquw</t>
+  </si>
+  <si>
+    <t>Dimension/Facr</t>
+  </si>
+  <si>
+    <t>No Visitrs</t>
+  </si>
+  <si>
+    <t>WH</t>
+  </si>
+  <si>
+    <t>Visits</t>
+  </si>
+  <si>
+    <t>FieldSession</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Filter Condition - N</t>
+  </si>
+  <si>
+    <t>No Searches</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N </t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>Ops</t>
   </si>
 </sst>
 </file>
@@ -1132,10 +1215,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1147,18 +1230,18 @@
     <col min="6" max="6" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1166,7 +1249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -1177,7 +1260,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1187,8 +1270,11 @@
       <c r="F6" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1198,17 +1284,14 @@
       <c r="F7" t="s">
         <v>77</v>
       </c>
+      <c r="L7" t="s">
+        <v>10</v>
+      </c>
       <c r="M7" t="s">
-        <v>9</v>
-      </c>
-      <c r="N7" t="s">
-        <v>10</v>
-      </c>
-      <c r="O7" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1218,22 +1301,22 @@
       <c r="E8" t="s">
         <v>4</v>
       </c>
-      <c r="O8" t="s">
+      <c r="M8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
       <c r="E9" t="s">
         <v>5</v>
       </c>
-      <c r="O9" t="s">
+      <c r="M9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1241,7 +1324,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1249,7 +1332,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>12</v>
       </c>
@@ -1266,12 +1349,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="E16" t="s">
         <v>37</v>
@@ -1327,7 +1410,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5381,9 +5464,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I57" sqref="I57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7767,10 +7850,188 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>130</v>
+      </c>
+      <c r="I4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" t="s">
+        <v>149</v>
+      </c>
+      <c r="I1" t="s">
+        <v>152</v>
+      </c>
+      <c r="J1" t="s">
+        <v>153</v>
+      </c>
+      <c r="K1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I2" t="s">
+        <v>152</v>
+      </c>
+      <c r="J2" t="s">
+        <v>153</v>
+      </c>
+      <c r="K2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>150</v>
+      </c>
+      <c r="I3" t="s">
+        <v>152</v>
+      </c>
+      <c r="J3" t="s">
+        <v>153</v>
+      </c>
+      <c r="K3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>151</v>
+      </c>
+      <c r="J4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated Ins Understanding & server.r
</commit_message>
<xml_diff>
--- a/Insurance Understanding.xlsx
+++ b/Insurance Understanding.xlsx
@@ -5,21 +5,22 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arun\Documents\GitHub\Insurance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Reporting\Insurance Reporting Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7035" activeTab="6"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Discussion" sheetId="1" r:id="rId1"/>
     <sheet name="TLI" sheetId="3" r:id="rId2"/>
     <sheet name="CI" sheetId="4" r:id="rId3"/>
     <sheet name="HI" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="6" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="7" r:id="rId6"/>
+    <sheet name="Dimentions" sheetId="6" r:id="rId5"/>
+    <sheet name="Data Captured" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -302,8 +303,384 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Arun Peter</author>
+  </authors>
+  <commentList>
+    <comment ref="E31" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Arun Peter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+New or Topup</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E32" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Arun Peter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Individual or Floater</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E35" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Arun Peter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Annual currently for all partners.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D49" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Arun Peter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Some Partners</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D50" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Arun Peter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Some Partners</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D52" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Arun Peter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Some Partners</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E60" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Arun Peter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Optional</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E61" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Arun Peter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Optional</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C62" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Arun Peter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Some Partners</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E78" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Arun Peter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Some Partners
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E79" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Arun Peter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Some Partners
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E80" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Arun Peter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Some Partners
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E82" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Arun Peter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Some Partners
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E84" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Arun Peter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Some Partners
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E85" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Arun Peter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Some Partners
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1988" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2397" uniqueCount="264">
   <si>
     <t>visit</t>
   </si>
@@ -689,54 +1066,15 @@
     <t xml:space="preserve">process understanding </t>
   </si>
   <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Smoke/</t>
-  </si>
-  <si>
     <t>Applicant City</t>
   </si>
   <si>
-    <t>Gross Mn</t>
-  </si>
-  <si>
     <t>CI</t>
   </si>
   <si>
     <t>TLI</t>
   </si>
   <si>
-    <t>Dimensions at eligibiity Page</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>Appl Dimension</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date of </t>
-  </si>
-  <si>
-    <t>na</t>
-  </si>
-  <si>
-    <t>Raise Reqest</t>
-  </si>
-  <si>
-    <t>First</t>
-  </si>
-  <si>
-    <t>uniquw</t>
-  </si>
-  <si>
-    <t>Dimension/Facr</t>
-  </si>
-  <si>
     <t>No Visitrs</t>
   </si>
   <si>
@@ -746,21 +1084,12 @@
     <t>Visits</t>
   </si>
   <si>
-    <t>FieldSession</t>
-  </si>
-  <si>
     <t>Sum</t>
   </si>
   <si>
-    <t>Filter Condition - N</t>
-  </si>
-  <si>
     <t>No Searches</t>
   </si>
   <si>
-    <t xml:space="preserve">N </t>
-  </si>
-  <si>
     <t>Finance</t>
   </si>
   <si>
@@ -768,13 +1097,388 @@
   </si>
   <si>
     <t>Ops</t>
+  </si>
+  <si>
+    <t>Adults 1|2</t>
+  </si>
+  <si>
+    <t>How old is the eldest member to be insured?</t>
+  </si>
+  <si>
+    <t>18-99+</t>
+  </si>
+  <si>
+    <t>Does your employer provide HI</t>
+  </si>
+  <si>
+    <t>Members to Insure - Adult</t>
+  </si>
+  <si>
+    <t>Members to Insure - Child</t>
+  </si>
+  <si>
+    <t>0-4</t>
+  </si>
+  <si>
+    <t>0-10L | Ignore</t>
+  </si>
+  <si>
+    <t>Dimension/Fact</t>
+  </si>
+  <si>
+    <t>Dimentions at Offer Page</t>
+  </si>
+  <si>
+    <t>Tenure</t>
+  </si>
+  <si>
+    <t>Coverage Type</t>
+  </si>
+  <si>
+    <t>Critical Factors</t>
+  </si>
+  <si>
+    <t>Premium incl taxes</t>
+  </si>
+  <si>
+    <t>Cost per Day</t>
+  </si>
+  <si>
+    <t>Coverage Highlights</t>
+  </si>
+  <si>
+    <t>Product Brochure</t>
+  </si>
+  <si>
+    <t>Policy Wordings</t>
+  </si>
+  <si>
+    <t>Accessories included</t>
+  </si>
+  <si>
+    <t>Add On</t>
+  </si>
+  <si>
+    <t>Garage List</t>
+  </si>
+  <si>
+    <t>Cliam Form</t>
+  </si>
+  <si>
+    <t>Discounts Eligibility/Applied</t>
+  </si>
+  <si>
+    <t>Extra Cover Opted</t>
+  </si>
+  <si>
+    <t>Monlthly Payout option</t>
+  </si>
+  <si>
+    <t>Premium Frequency</t>
+  </si>
+  <si>
+    <t>Total Payout</t>
+  </si>
+  <si>
+    <t>Coverage Amt/Insured Value/Lump Sum</t>
+  </si>
+  <si>
+    <t>Claim Settlement Ratio</t>
+  </si>
+  <si>
+    <t>Premium for New Buyers</t>
+  </si>
+  <si>
+    <t>Max maturity Age</t>
+  </si>
+  <si>
+    <t>Grievances Resolved</t>
+  </si>
+  <si>
+    <t>Optional Q-Higher Voluntary Deduction, DOB, Occupation, anti-theft device, Member AAI (compulsory)</t>
+  </si>
+  <si>
+    <t>Special/Good to Have Features</t>
+  </si>
+  <si>
+    <t>Accidental Death Benefit</t>
+  </si>
+  <si>
+    <t>Dimensions at Eligibity Page</t>
+  </si>
+  <si>
+    <t>Filter Condition</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>SessionCount</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>DB</t>
+  </si>
+  <si>
+    <t>Metric</t>
+  </si>
+  <si>
+    <t>Used by Teams</t>
+  </si>
+  <si>
+    <t>Offers</t>
+  </si>
+  <si>
+    <t>Unique</t>
+  </si>
+  <si>
+    <t>Fact</t>
+  </si>
+  <si>
+    <t>Dimention</t>
+  </si>
+  <si>
+    <t>NCB %</t>
+  </si>
+  <si>
+    <t>Dimension</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Eligibility</t>
+  </si>
+  <si>
+    <t>Annual Income (Gross Annual Income) Needs More Investigation</t>
+  </si>
+  <si>
+    <t>WH Availability</t>
+  </si>
+  <si>
+    <t>FieldName</t>
+  </si>
+  <si>
+    <t>Partner Name</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Marital Status</t>
+  </si>
+  <si>
+    <t>Are you a Politically Exposed Person</t>
+  </si>
+  <si>
+    <t>Policy Type</t>
+  </si>
+  <si>
+    <t>Dimensions at App Page</t>
+  </si>
+  <si>
+    <t>PAN</t>
+  </si>
+  <si>
+    <t>Age/DOB</t>
+  </si>
+  <si>
+    <t>Insured Person Gender</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Already Cancer/Kidney/Heart/Psychatric Problem</t>
+  </si>
+  <si>
+    <t>Pre-Condition</t>
+  </si>
+  <si>
+    <t>BPL/Disabled/Unorg Sector</t>
+  </si>
+  <si>
+    <t>Hospitalized &lt;4Yrs</t>
+  </si>
+  <si>
+    <t>Claimed in Past or Present Ins</t>
+  </si>
+  <si>
+    <t>Has ever Changed/Cancelled/Declined</t>
+  </si>
+  <si>
+    <t>Nominee Name</t>
+  </si>
+  <si>
+    <t>Nominee Relation</t>
+  </si>
+  <si>
+    <t>Occupation</t>
+  </si>
+  <si>
+    <t>Qualification</t>
+  </si>
+  <si>
+    <t>Alcohol/Smoking/Tobacco/Narcotics</t>
+  </si>
+  <si>
+    <t>Nominee DOB</t>
+  </si>
+  <si>
+    <t>Nominee Mobile</t>
+  </si>
+  <si>
+    <t>Nationality</t>
+  </si>
+  <si>
+    <t>Industry Type</t>
+  </si>
+  <si>
+    <t>Employer Name</t>
+  </si>
+  <si>
+    <t>Nominee Gender</t>
+  </si>
+  <si>
+    <t>Place of Birth</t>
+  </si>
+  <si>
+    <t>NRI</t>
+  </si>
+  <si>
+    <t>Electronic Insurance Account</t>
+  </si>
+  <si>
+    <t>Payment Method</t>
+  </si>
+  <si>
+    <t>Special Industry</t>
+  </si>
+  <si>
+    <t>Occupational Hazards</t>
+  </si>
+  <si>
+    <t>Number of Nominees</t>
+  </si>
+  <si>
+    <t>Car Manufactured YYMM</t>
+  </si>
+  <si>
+    <t>Insurance Expiry Date</t>
+  </si>
+  <si>
+    <t>Before going into the App Page</t>
+  </si>
+  <si>
+    <t>Registration No</t>
+  </si>
+  <si>
+    <t>Chasis No</t>
+  </si>
+  <si>
+    <t>Engine No</t>
+  </si>
+  <si>
+    <t>Previous Policy No</t>
+  </si>
+  <si>
+    <t>Is the Car Financed</t>
+  </si>
+  <si>
+    <t>Car Ownership Change in LTM (12mth)</t>
+  </si>
+  <si>
+    <t>Offer</t>
+  </si>
+  <si>
+    <t>App</t>
+  </si>
+  <si>
+    <t>Premium excl taxes</t>
+  </si>
+  <si>
+    <t>Car Model</t>
+  </si>
+  <si>
+    <t>Car First Registerd Date</t>
+  </si>
+  <si>
+    <t>MP Ins</t>
+  </si>
+  <si>
+    <t>MP</t>
+  </si>
+  <si>
+    <t>option to segrageate</t>
+  </si>
+  <si>
+    <t>segregate it as a dimention</t>
+  </si>
+  <si>
+    <t>Cummulative</t>
+  </si>
+  <si>
+    <t>visits</t>
+  </si>
+  <si>
+    <t>searches</t>
+  </si>
+  <si>
+    <t>DWH download</t>
+  </si>
+  <si>
+    <t>preprocess</t>
+  </si>
+  <si>
+    <t>aggregate</t>
+  </si>
+  <si>
+    <t>master join</t>
+  </si>
+  <si>
+    <t>SOS</t>
+  </si>
+  <si>
+    <t>join with Apps</t>
+  </si>
+  <si>
+    <t>get income bucket, etc and backfill in Searches * Offers</t>
+  </si>
+  <si>
+    <t>Offer waterfall</t>
+  </si>
+  <si>
+    <t>leads</t>
+  </si>
+  <si>
+    <t>appscreated</t>
+  </si>
+  <si>
+    <t>mobile count</t>
+  </si>
+  <si>
+    <t>created dt</t>
+  </si>
+  <si>
+    <t>effective created dt</t>
+  </si>
+  <si>
+    <t>flags</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -802,6 +1506,14 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="15">
@@ -902,7 +1614,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -929,6 +1641,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1217,9 +1930,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1409,8 +2120,8 @@
   <dimension ref="A1:H195"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <pane ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G171" sqref="G171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5464,9 +6175,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B46" sqref="B46"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7848,97 +8559,1592 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="3" width="24" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I97"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C37" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B54" sqref="B54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="59.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B7" t="s">
+        <v>191</v>
+      </c>
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>190</v>
+      </c>
+      <c r="B9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>190</v>
+      </c>
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>190</v>
+      </c>
+      <c r="B11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>190</v>
+      </c>
+      <c r="B12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>190</v>
+      </c>
+      <c r="B14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>190</v>
+      </c>
+      <c r="B15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>190</v>
+      </c>
+      <c r="B16" t="s">
+        <v>109</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>190</v>
+      </c>
+      <c r="B17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>190</v>
+      </c>
+      <c r="B18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>190</v>
+      </c>
+      <c r="B19" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>190</v>
+      </c>
+      <c r="B20" t="s">
+        <v>187</v>
+      </c>
+      <c r="D20" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>190</v>
+      </c>
+      <c r="B21" t="s">
+        <v>143</v>
+      </c>
+      <c r="E21" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>190</v>
+      </c>
+      <c r="B22" t="s">
+        <v>144</v>
+      </c>
+      <c r="E22" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B23" t="s">
+        <v>140</v>
+      </c>
+      <c r="E23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>190</v>
+      </c>
+      <c r="B24" t="s">
+        <v>142</v>
+      </c>
+      <c r="E24" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>238</v>
+      </c>
+      <c r="B27" t="s">
+        <v>194</v>
+      </c>
+      <c r="C27" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" t="s">
+        <v>46</v>
+      </c>
+      <c r="E27" t="s">
+        <v>46</v>
+      </c>
+      <c r="F27" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>238</v>
+      </c>
+      <c r="B28" t="s">
+        <v>166</v>
+      </c>
+      <c r="C28" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>238</v>
+      </c>
+      <c r="B29" t="s">
+        <v>163</v>
+      </c>
+      <c r="C29" t="s">
+        <v>46</v>
+      </c>
+      <c r="F29" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>238</v>
+      </c>
+      <c r="B30" t="s">
+        <v>149</v>
+      </c>
+      <c r="C30" t="s">
+        <v>46</v>
+      </c>
+      <c r="E30" t="s">
+        <v>46</v>
+      </c>
+      <c r="F30" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>238</v>
+      </c>
+      <c r="B31" t="s">
+        <v>150</v>
+      </c>
+      <c r="C31" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" t="s">
+        <v>46</v>
+      </c>
+      <c r="F31" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>238</v>
+      </c>
+      <c r="B32" t="s">
+        <v>198</v>
+      </c>
+      <c r="E32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>238</v>
+      </c>
+      <c r="B33" t="s">
+        <v>152</v>
+      </c>
+      <c r="C33" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" t="s">
+        <v>46</v>
+      </c>
+      <c r="E33" t="s">
+        <v>46</v>
+      </c>
+      <c r="F33" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>238</v>
+      </c>
+      <c r="B35" t="s">
+        <v>164</v>
+      </c>
+      <c r="C35" t="s">
+        <v>46</v>
+      </c>
+      <c r="E35" t="s">
+        <v>46</v>
+      </c>
+      <c r="F35" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>238</v>
+      </c>
+      <c r="B36" t="s">
+        <v>157</v>
+      </c>
+      <c r="D36" t="s">
+        <v>46</v>
+      </c>
+      <c r="F36" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>238</v>
+      </c>
+      <c r="B37" t="s">
+        <v>158</v>
+      </c>
+      <c r="C37" t="s">
+        <v>46</v>
+      </c>
+      <c r="D37" t="s">
+        <v>46</v>
+      </c>
+      <c r="F37" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>238</v>
+      </c>
+      <c r="B38" t="s">
+        <v>167</v>
+      </c>
+      <c r="C38" t="s">
+        <v>46</v>
+      </c>
+      <c r="F38" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>238</v>
+      </c>
+      <c r="B39" t="s">
+        <v>153</v>
+      </c>
+      <c r="C39" t="s">
+        <v>46</v>
+      </c>
+      <c r="E39" t="s">
+        <v>46</v>
+      </c>
+      <c r="F39" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>238</v>
+      </c>
+      <c r="B40" t="s">
+        <v>165</v>
+      </c>
+      <c r="C40" t="s">
+        <v>46</v>
+      </c>
+      <c r="F40" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>238</v>
+      </c>
+      <c r="B41" t="s">
+        <v>151</v>
+      </c>
+      <c r="C41" t="s">
+        <v>46</v>
+      </c>
+      <c r="E41" t="s">
+        <v>46</v>
+      </c>
+      <c r="F41" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>238</v>
+      </c>
+      <c r="B42" t="s">
+        <v>154</v>
+      </c>
+      <c r="C42" t="s">
+        <v>46</v>
+      </c>
+      <c r="D42" t="s">
+        <v>46</v>
+      </c>
+      <c r="E42" t="s">
+        <v>46</v>
+      </c>
+      <c r="F42" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>238</v>
+      </c>
+      <c r="B43" t="s">
+        <v>161</v>
+      </c>
+      <c r="D43" t="s">
+        <v>46</v>
+      </c>
+      <c r="F43" t="s">
+        <v>188</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>238</v>
+      </c>
+      <c r="B44" t="s">
+        <v>162</v>
+      </c>
+      <c r="D44" t="s">
+        <v>46</v>
+      </c>
+      <c r="F44" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>238</v>
+      </c>
+      <c r="B45" t="s">
+        <v>170</v>
+      </c>
+      <c r="C45" t="s">
+        <v>46</v>
+      </c>
+      <c r="F45" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>238</v>
+      </c>
+      <c r="B46" t="s">
+        <v>168</v>
+      </c>
+      <c r="C46" t="s">
+        <v>46</v>
+      </c>
+      <c r="F46" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>238</v>
+      </c>
+      <c r="B47" t="s">
+        <v>169</v>
+      </c>
+      <c r="C47" t="s">
+        <v>46</v>
+      </c>
+      <c r="F47" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>238</v>
+      </c>
+      <c r="B48" t="s">
+        <v>172</v>
+      </c>
+      <c r="C48" t="s">
+        <v>46</v>
+      </c>
+      <c r="E48" t="s">
+        <v>46</v>
+      </c>
+      <c r="F48" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>238</v>
+      </c>
+      <c r="B49" t="s">
+        <v>155</v>
+      </c>
+      <c r="C49" t="s">
+        <v>46</v>
+      </c>
+      <c r="D49" t="s">
+        <v>46</v>
+      </c>
+      <c r="E49" t="s">
+        <v>46</v>
+      </c>
+      <c r="F49" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>238</v>
+      </c>
+      <c r="B50" t="s">
+        <v>156</v>
+      </c>
+      <c r="C50" t="s">
+        <v>46</v>
+      </c>
+      <c r="D50" t="s">
+        <v>46</v>
+      </c>
+      <c r="E50" t="s">
+        <v>46</v>
+      </c>
+      <c r="F50" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>238</v>
+      </c>
+      <c r="B51" t="s">
+        <v>173</v>
+      </c>
+      <c r="C51" t="s">
+        <v>46</v>
+      </c>
+      <c r="F51" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>238</v>
+      </c>
+      <c r="B52" t="s">
+        <v>159</v>
+      </c>
+      <c r="D52" t="s">
+        <v>46</v>
+      </c>
+      <c r="F52" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>238</v>
+      </c>
+      <c r="B53" t="s">
+        <v>160</v>
+      </c>
+      <c r="D53" t="s">
+        <v>46</v>
+      </c>
+      <c r="F53" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>238</v>
+      </c>
+      <c r="B54" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="D54" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>238</v>
+      </c>
+      <c r="B55" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="D55" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>238</v>
+      </c>
+      <c r="B56" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="D56" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>239</v>
+      </c>
+      <c r="B59" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="D59" s="22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>239</v>
+      </c>
+      <c r="B60" t="s">
+        <v>48</v>
+      </c>
+      <c r="C60" s="10"/>
+      <c r="E60" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>239</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F61" s="10"/>
+    </row>
+    <row r="62" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>239</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D62" s="10"/>
+      <c r="E62" s="10"/>
+      <c r="F62" s="10"/>
+    </row>
+    <row r="63" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>239</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F63" s="10"/>
+    </row>
+    <row r="64" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>239</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D64" s="10"/>
+      <c r="E64" s="10"/>
+      <c r="F64" s="10"/>
+    </row>
+    <row r="65" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>239</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="C65" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D65" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F65" s="10"/>
+    </row>
+    <row r="66" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>239</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="C66" s="10"/>
+      <c r="D66" s="10"/>
+      <c r="E66" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F66" s="10"/>
+    </row>
+    <row r="67" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>239</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="C67" s="10"/>
+      <c r="D67" s="10"/>
+      <c r="E67" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F67" s="10"/>
+    </row>
+    <row r="68" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>239</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="C68" s="10"/>
+      <c r="D68" s="10"/>
+      <c r="E68" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F68" s="10"/>
+    </row>
+    <row r="69" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>239</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C69" s="10"/>
+      <c r="D69" s="10"/>
+      <c r="E69" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F69" s="10"/>
+    </row>
+    <row r="70" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>239</v>
+      </c>
+      <c r="B70" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="C70" s="10"/>
+      <c r="D70" s="10"/>
+      <c r="E70" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F70" s="10"/>
+    </row>
+    <row r="71" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>239</v>
+      </c>
+      <c r="B71" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
+      <c r="E71" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F71" s="10"/>
+    </row>
+    <row r="72" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>239</v>
+      </c>
+      <c r="B72" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="C72" s="10"/>
+      <c r="D72" s="10"/>
+      <c r="E72" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F72" s="10"/>
+    </row>
+    <row r="73" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>239</v>
+      </c>
+      <c r="B73" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
+      <c r="E73" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F73" s="10"/>
+    </row>
+    <row r="74" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>239</v>
+      </c>
+      <c r="B74" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="C74" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D74" s="10"/>
+      <c r="E74" s="10"/>
+      <c r="F74" s="10"/>
+    </row>
+    <row r="75" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>239</v>
+      </c>
+      <c r="B75" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="C75" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D75" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E75" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F75" s="10"/>
+    </row>
+    <row r="76" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>239</v>
+      </c>
+      <c r="B76" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="C76" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E76" s="10"/>
+      <c r="F76" s="10"/>
+    </row>
+    <row r="77" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>239</v>
+      </c>
+      <c r="B77" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="C77" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D77" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E77" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F77" s="10"/>
+    </row>
+    <row r="78" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>239</v>
+      </c>
+      <c r="B78" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="C78" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D78" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E78" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F78" s="10"/>
+    </row>
+    <row r="79" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>239</v>
+      </c>
+      <c r="B79" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="C79" s="10"/>
+      <c r="D79" s="10"/>
+      <c r="E79" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F79" s="10"/>
+    </row>
+    <row r="80" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>239</v>
+      </c>
+      <c r="B80" t="s">
+        <v>196</v>
+      </c>
+      <c r="C80" t="s">
+        <v>46</v>
+      </c>
+      <c r="E80" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>239</v>
+      </c>
+      <c r="B81" t="s">
+        <v>220</v>
+      </c>
+      <c r="C81" t="s">
+        <v>46</v>
+      </c>
+      <c r="E81" s="10"/>
+    </row>
+    <row r="82" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>239</v>
+      </c>
+      <c r="B82" t="s">
+        <v>213</v>
+      </c>
+      <c r="C82" t="s">
+        <v>46</v>
+      </c>
+      <c r="D82" t="s">
+        <v>46</v>
+      </c>
+      <c r="E82" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>239</v>
+      </c>
+      <c r="B83" t="s">
+        <v>219</v>
+      </c>
+      <c r="C83" t="s">
+        <v>46</v>
+      </c>
+      <c r="E83" s="10"/>
+    </row>
+    <row r="84" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>239</v>
+      </c>
+      <c r="B84" t="s">
+        <v>214</v>
+      </c>
+      <c r="C84" t="s">
+        <v>46</v>
+      </c>
+      <c r="E84" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>239</v>
+      </c>
+      <c r="B85" t="s">
+        <v>215</v>
+      </c>
+      <c r="E85" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>239</v>
+      </c>
+      <c r="B86" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="C86" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D86" s="10"/>
+      <c r="E86" s="10"/>
+      <c r="F86" s="10"/>
+    </row>
+    <row r="87" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>239</v>
+      </c>
+      <c r="B87" t="s">
+        <v>197</v>
+      </c>
+      <c r="C87" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>239</v>
+      </c>
+      <c r="B88" t="s">
+        <v>226</v>
+      </c>
+      <c r="C88" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>239</v>
+      </c>
+      <c r="B89" t="s">
+        <v>227</v>
+      </c>
+      <c r="C89" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>239</v>
+      </c>
+      <c r="B90" t="s">
+        <v>224</v>
+      </c>
+      <c r="C90" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>239</v>
+      </c>
+      <c r="B91" t="s">
+        <v>236</v>
+      </c>
+      <c r="D91" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>239</v>
+      </c>
+      <c r="B92" t="s">
+        <v>237</v>
+      </c>
+      <c r="D92" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>239</v>
+      </c>
+      <c r="B93" t="s">
+        <v>232</v>
+      </c>
+      <c r="D93" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>239</v>
+      </c>
+      <c r="B94" t="s">
+        <v>233</v>
+      </c>
+      <c r="D94" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>239</v>
+      </c>
+      <c r="B95" t="s">
+        <v>234</v>
+      </c>
+      <c r="D95" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>239</v>
+      </c>
+      <c r="B96" t="s">
+        <v>235</v>
+      </c>
+      <c r="D96" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>239</v>
+      </c>
+      <c r="B97" t="s">
+        <v>225</v>
+      </c>
+      <c r="D97" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E2" t="s">
         <v>134</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" t="s">
+        <v>136</v>
+      </c>
+      <c r="J2" t="s">
+        <v>137</v>
+      </c>
+      <c r="K2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" t="s">
         <v>132</v>
       </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="C3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E3" t="s">
+        <v>184</v>
+      </c>
+      <c r="I3" t="s">
+        <v>136</v>
+      </c>
+      <c r="J3" t="s">
+        <v>137</v>
+      </c>
+      <c r="K3" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>129</v>
-      </c>
-      <c r="F3" t="s">
-        <v>139</v>
-      </c>
-      <c r="G3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>123</v>
+      </c>
+      <c r="B4" t="s">
+        <v>132</v>
       </c>
       <c r="I4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
         <v>136</v>
       </c>
-      <c r="D6" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="J4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>141</v>
+      <c r="K4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>132</v>
+      </c>
+      <c r="J5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -7946,89 +10152,110 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="B2:P17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E1" t="s">
-        <v>148</v>
-      </c>
-      <c r="F1" t="s">
-        <v>149</v>
-      </c>
-      <c r="I1" t="s">
-        <v>152</v>
-      </c>
-      <c r="J1" t="s">
-        <v>153</v>
-      </c>
-      <c r="K1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>123</v>
-      </c>
-      <c r="I2" t="s">
-        <v>152</v>
-      </c>
-      <c r="J2" t="s">
-        <v>153</v>
-      </c>
-      <c r="K2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>150</v>
-      </c>
-      <c r="I3" t="s">
-        <v>152</v>
-      </c>
-      <c r="J3" t="s">
-        <v>153</v>
-      </c>
-      <c r="K3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>151</v>
-      </c>
-      <c r="J4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K5" t="s">
-        <v>154</v>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>254</v>
+      </c>
+      <c r="G6" t="s">
+        <v>255</v>
+      </c>
+      <c r="J6" t="s">
+        <v>257</v>
+      </c>
+      <c r="M6" t="s">
+        <v>258</v>
+      </c>
+      <c r="O6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>248</v>
+      </c>
+      <c r="D7" t="s">
+        <v>249</v>
+      </c>
+      <c r="F7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>250</v>
+      </c>
+      <c r="M8" t="s">
+        <v>260</v>
+      </c>
+      <c r="O8" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>251</v>
+      </c>
+      <c r="G9" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="P14" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="P15" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="17" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P17" t="s">
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>